<commit_message>
Update, push all the code so that Sara can access it
</commit_message>
<xml_diff>
--- a/data/NOMAL.xlsx
+++ b/data/NOMAL.xlsx
@@ -716,13 +716,16 @@
   </sheetPr>
   <dimension ref="A1:EA75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DS9" activeCellId="0" sqref="DS9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CS1" activeCellId="0" sqref="CS1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="45.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="0" width="12.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,7 +1120,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>3761</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>35319</v>
       </c>
@@ -2513,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>133</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>5349</v>
       </c>
@@ -20006,7 +20009,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -20029,7 +20032,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>